<commit_message>
add river inspection form
</commit_message>
<xml_diff>
--- a/Dimagi/Form contents CC Apps for Ento Data Collection (002).xlsx
+++ b/Dimagi/Form contents CC Apps for Ento Data Collection (002).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\Dimagi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bonhe\Repositories\dsa-forms\Dimagi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2E2229-7EA5-493E-AC1C-C7ACAE8D3406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE663AC2-6C67-493D-930C-7F7B505B4C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="River Prospection" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="189">
   <si>
     <t>Form in English</t>
   </si>
@@ -615,6 +615,9 @@
   </si>
   <si>
     <t>Not necessary</t>
+  </si>
+  <si>
+    <t>Need recorder Id Forms</t>
   </si>
 </sst>
 </file>
@@ -899,6 +902,7 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -920,7 +924,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -1142,26 +1145,26 @@
   </sheetPr>
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="18.140625" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="34"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="35"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -1172,14 +1175,14 @@
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="38"/>
     </row>
     <row r="4" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
@@ -1298,7 +1301,7 @@
       <c r="F10" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="43" t="s">
+      <c r="G10" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -1383,24 +1386,27 @@
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-    </row>
-    <row r="17" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+    </row>
+    <row r="17" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="32" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>47</v>
       </c>
@@ -1416,7 +1422,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>49</v>
       </c>
@@ -1434,7 +1440,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>51</v>
       </c>
@@ -1452,7 +1458,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>31</v>
       </c>
@@ -1470,7 +1476,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>53</v>
       </c>
@@ -1490,7 +1496,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>55</v>
       </c>
@@ -1508,7 +1514,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>57</v>
       </c>
@@ -1526,7 +1532,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>61</v>
       </c>
@@ -1544,7 +1550,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>65</v>
       </c>
@@ -1562,7 +1568,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>69</v>
       </c>
@@ -1580,7 +1586,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>72</v>
       </c>
@@ -1598,7 +1604,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>75</v>
       </c>
@@ -1616,7 +1622,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>77</v>
       </c>
@@ -1634,7 +1640,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>79</v>
       </c>
@@ -1650,7 +1656,7 @@
       </c>
       <c r="F31" s="10"/>
     </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>82</v>
       </c>
@@ -1755,14 +1761,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="37"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
@@ -1773,14 +1779,14 @@
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="42"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="43"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
@@ -2091,14 +2097,14 @@
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="40" t="s">
+      <c r="A24" s="41" t="s">
         <v>140</v>
       </c>
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="42"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="43"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
@@ -2289,14 +2295,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="37"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
@@ -2307,14 +2313,14 @@
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="41" t="s">
         <v>155</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="42"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="43"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">

</xml_diff>